<commit_message>
Issue related to not vehicle detection solved
The sunday and saturday many agents do not leave home
</commit_message>
<xml_diff>
--- a/system/system_management.xlsx
+++ b/system/system_management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asier.divasson\Documents\GitHub\CogniCity\system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3B575F-0E0B-44F4-A013-15BF6AB0A483}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC19226-F8A4-4493-8BCB-FC1BA6B28535}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
   <si>
     <t>archetypes</t>
   </si>
@@ -109,9 +109,6 @@
   </si>
   <si>
     <t>building</t>
-  </si>
-  <si>
-    <t>noon_close</t>
   </si>
   <si>
     <t>false</t>
@@ -459,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="J2" sqref="J2:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -475,7 +472,7 @@
     <col min="6" max="6" width="6.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -495,25 +492,22 @@
         <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>31</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -532,27 +526,23 @@
       <c r="F2" t="s">
         <v>26</v>
       </c>
-      <c r="G2">
-        <f>13*60</f>
-        <v>780</v>
+      <c r="G2" t="s">
+        <v>28</v>
       </c>
       <c r="H2" t="s">
         <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -572,7 +562,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -589,7 +579,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -603,7 +593,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -617,7 +607,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>14</v>
       </c>
@@ -628,7 +618,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>14</v>
       </c>
@@ -639,7 +629,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>14</v>
       </c>
@@ -650,7 +640,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>17</v>
       </c>

</xml_diff>